<commit_message>
Update Formula and Sample HTML Report Before Running Test
</commit_message>
<xml_diff>
--- a/Active Data/TD_Rekomendasi Harga.xlsx
+++ b/Active Data/TD_Rekomendasi Harga.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F110E8A7-30EF-42F5-9F52-DA733FBBDC56}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC_Rekomendasi Harga" sheetId="1" r:id="rId1"/>
     <sheet name="DDT_Rekomendasi Harga" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,23 +422,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.1796875" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
-    <col min="3" max="3" width="24.26953125" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -453,7 +452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -467,7 +466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -481,7 +480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -493,7 +492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -505,7 +504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -513,7 +512,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -533,23 +532,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4163B86-B56B-4510-89EC-F5151B5AD3C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.36328125" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="19.08984375" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" customWidth="1"/>
-    <col min="5" max="5" width="24.26953125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -566,7 +565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -583,7 +582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -594,13 +593,13 @@
         <v>10000000</v>
       </c>
       <c r="D3" s="3">
-        <v>50000000</v>
+        <v>5000000</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -611,7 +610,7 @@
         <v>50000000</v>
       </c>
       <c r="D4" s="3">
-        <v>20000000</v>
+        <v>2000000</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>10</v>

</xml_diff>